<commit_message>
Added report, updated finetuning
</commit_message>
<xml_diff>
--- a/results/gpt-4o-mini_few-shot_ranking_scores_2025-04-12-12-02.xlsx
+++ b/results/gpt-4o-mini_few-shot_ranking_scores_2025-04-12-12-02.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/643fca571bbd5a59/Dokumente/adaptive-text-gen/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921ED9E7B8E10792D4C51CD0DC4925C3AB02F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{959B35D6-A4A2-4676-8080-FDA97E86D443}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -87,8 +93,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,24 +146,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +212,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -229,6 +246,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -263,9 +281,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,14 +457,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -485,7 +506,7 @@
         <v>37.64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -499,7 +520,7 @@
         <v>13.6</v>
       </c>
       <c r="E3">
-        <v>39.37</v>
+        <v>39.369999999999997</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -508,7 +529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -519,7 +540,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E4">
         <v>13.07</v>
@@ -531,14 +552,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D5">
@@ -554,7 +575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -577,7 +598,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -591,7 +612,7 @@
         <v>20.6</v>
       </c>
       <c r="E7">
-        <v>-0.57</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>

</xml_diff>